<commit_message>
modified:   dataset/descriptions/hypercarge_locations.xlsx 	modified:   dataset/task_1/hypercarge_locations_task1.csv
</commit_message>
<xml_diff>
--- a/dataset/descriptions/hypercarge_locations.xlsx
+++ b/dataset/descriptions/hypercarge_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autostrade-my.sharepoint.com/personal/george_son_freeto-x_it/Documents/Eventi/Luiss/dataset_desc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\charging_stations\dataset\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC1048ABE15E58CC5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2609D541-6F5D-44DE-AFE3-7BAA52FF9080}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA947C-DA6B-411B-96D3-84D200512262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -888,18 +888,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -921,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -932,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -943,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -954,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -965,7 +965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -976,7 +976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -987,7 +987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -998,7 +998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>62</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>64</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>66</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>68</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>70</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>72</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>74</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>76</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>78</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>81</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>83</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>85</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>87</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>89</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>91</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>93</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>95</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>97</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>99</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>101</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>103</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>105</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>107</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>109</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>111</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>113</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>115</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>117</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>119</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>121</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>123</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>125</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>127</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>129</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>131</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>133</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>135</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>137</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>139</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>141</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>143</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>145</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>147</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>149</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>151</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>153</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>155</v>
       </c>

</xml_diff>